<commit_message>
Modifications in the output
</commit_message>
<xml_diff>
--- a/Matenimiento/data_out.xlsx
+++ b/Matenimiento/data_out.xlsx
@@ -553,10 +553,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.521894093686354</v>
+        <v>0.525288526816022</v>
       </c>
       <c r="F2">
-        <v>0.946030451332246</v>
+        <v>0.945350734094617</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -568,64 +568,64 @@
         <v>0.000596658711217184</v>
       </c>
       <c r="J2">
-        <v>0.0217391304347826</v>
+        <v>0.0072463768115942</v>
       </c>
       <c r="K2">
-        <v>0.209259259259259</v>
+        <v>0.193981481481481</v>
       </c>
       <c r="L2">
-        <v>0.969826056088037</v>
+        <v>0.963532356095817</v>
       </c>
       <c r="M2">
-        <v>0.871536523929471</v>
+        <v>0.845771144278607</v>
       </c>
       <c r="P2">
-        <v>35.7076794847022</v>
+        <v>38.5842981036431</v>
       </c>
       <c r="Q2">
-        <v>81.7416302921976</v>
+        <v>84.2261089565554</v>
       </c>
       <c r="R2">
-        <v>38.9160650447751</v>
+        <v>36.4842671200365</v>
       </c>
       <c r="S2">
-        <v>38.9724139925624</v>
+        <v>36.444452276668</v>
       </c>
       <c r="T2">
-        <v>96.1418566442795</v>
+        <v>94.68480666949</v>
       </c>
       <c r="U2">
-        <v>5.77172980963161</v>
+        <v>4.70990948609626</v>
       </c>
       <c r="V2">
-        <v>10.2582715210158</v>
+        <v>11.6424298078935</v>
       </c>
       <c r="W2">
-        <v>4.25561994302023</v>
+        <v>4.23926165985295</v>
       </c>
       <c r="X2">
-        <v>6.89476558976116</v>
+        <v>4.06213030060682</v>
       </c>
       <c r="Y2">
-        <v>12.1832424963237</v>
+        <v>11.1603131756513</v>
       </c>
       <c r="Z2">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA2">
         <v>9600</v>
       </c>
       <c r="AB2">
-        <v>403.915628143351</v>
+        <v>387.33756130081</v>
       </c>
       <c r="AC2">
-        <v>13476.10625</v>
+        <v>13496.1731944444</v>
       </c>
       <c r="AD2">
-        <v>7307.84534407887</v>
+        <v>7299.65216092141</v>
       </c>
       <c r="AE2">
-        <v>2292.15465592113</v>
+        <v>2300.34783907859</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -645,13 +645,13 @@
         <v>0.000339443312966735</v>
       </c>
       <c r="F3">
-        <v>0.205274605764002</v>
+        <v>0.210032626427406</v>
       </c>
       <c r="G3">
-        <v>0.461904761904762</v>
+        <v>0.507142857142857</v>
       </c>
       <c r="H3">
-        <v>0.992656449553001</v>
+        <v>0.999680715197957</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -663,64 +663,64 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.29490662139219</v>
+        <v>0.289473684210526</v>
       </c>
       <c r="M3">
-        <v>0.76958604173794</v>
+        <v>0.739287558079504</v>
       </c>
       <c r="N3">
-        <v>0.97787610619469</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0.695652173913043</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>32.0526190615534</v>
+        <v>34.4541272545617</v>
       </c>
       <c r="Q3">
-        <v>72.8041884467619</v>
+        <v>73.577675587252</v>
       </c>
       <c r="R3">
-        <v>33.7855997039402</v>
+        <v>33.0308755311829</v>
       </c>
       <c r="S3">
-        <v>34.8642388134045</v>
+        <v>31.8073515075635</v>
       </c>
       <c r="T3">
-        <v>85.2495899125926</v>
+        <v>84.3299492697222</v>
       </c>
       <c r="U3">
-        <v>4.104303401588</v>
+        <v>3.41241679533663</v>
       </c>
       <c r="V3">
-        <v>7.87185327076866</v>
+        <v>9.60524408162853</v>
       </c>
       <c r="W3">
-        <v>2.96850260565112</v>
+        <v>3.57101220662391</v>
       </c>
       <c r="X3">
-        <v>5.30867277759044</v>
+        <v>3.45252777291113</v>
       </c>
       <c r="Y3">
-        <v>8.9157228155766</v>
+        <v>8.98723844336624</v>
       </c>
       <c r="Z3">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA3">
         <v>19200</v>
       </c>
       <c r="AB3">
-        <v>416.847484153363</v>
+        <v>405.40939274852</v>
       </c>
       <c r="AC3">
-        <v>6946.02125</v>
+        <v>7009.50152777778</v>
       </c>
       <c r="AD3">
-        <v>13824.9984880689</v>
+        <v>13768.2519961404</v>
       </c>
       <c r="AE3">
-        <v>5375.00151193114</v>
+        <v>5431.74800385963</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.000339443312966735</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0.000407830342577488</v>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.74904214559387</v>
+        <v>0.752554278416347</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -758,64 +758,64 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.0617996604414261</v>
+        <v>0.0551595383570944</v>
       </c>
       <c r="M4">
-        <v>0.177886576907385</v>
+        <v>0.181694546443628</v>
       </c>
       <c r="N4">
         <v>0.102380952380952</v>
       </c>
       <c r="O4">
-        <v>0.297709923664122</v>
+        <v>0.292903225806452</v>
       </c>
       <c r="P4">
-        <v>31.2560119229898</v>
+        <v>33.2648156459609</v>
       </c>
       <c r="Q4">
-        <v>70.5867644284183</v>
+        <v>70.8879611879411</v>
       </c>
       <c r="R4">
-        <v>32.6960945624972</v>
+        <v>32.3006923372185</v>
       </c>
       <c r="S4">
-        <v>33.8435473447889</v>
+        <v>30.887821394275</v>
       </c>
       <c r="T4">
-        <v>82.7525070997425</v>
+        <v>82.2171261917537</v>
       </c>
       <c r="U4">
-        <v>3.86978899599299</v>
+        <v>3.19692489968859</v>
       </c>
       <c r="V4">
-        <v>7.62799082884691</v>
+        <v>9.26414868294762</v>
       </c>
       <c r="W4">
-        <v>2.71846647885635</v>
+        <v>3.48973551488594</v>
       </c>
       <c r="X4">
-        <v>4.94784441906502</v>
+        <v>3.36294078389247</v>
       </c>
       <c r="Y4">
-        <v>8.61781240588026</v>
+        <v>8.78865054319276</v>
       </c>
       <c r="Z4">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA4">
         <v>28800</v>
       </c>
       <c r="AB4">
-        <v>322.687046307654</v>
+        <v>314.697247910845</v>
       </c>
       <c r="AC4">
-        <v>3106.61736111111</v>
+        <v>3119.25388888889</v>
       </c>
       <c r="AD4">
-        <v>17758.5628148035</v>
+        <v>17749.2117798669</v>
       </c>
       <c r="AE4">
-        <v>11041.4371851965</v>
+        <v>11050.7882201331</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -835,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.000271886895051658</v>
+        <v>0.000135943447525829</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.131226053639847</v>
+        <v>0.127394636015326</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -853,64 +853,64 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.00407331975560081</v>
+        <v>0.00305498981670061</v>
       </c>
       <c r="M5">
-        <v>0.039026380201251</v>
+        <v>0.0375254928619986</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0.768099963248806</v>
+        <v>0.770581778265642</v>
       </c>
       <c r="P5">
-        <v>31.2296221607715</v>
+        <v>33.0792760551785</v>
       </c>
       <c r="Q5">
-        <v>70.3757406080006</v>
+        <v>70.6285069576724</v>
       </c>
       <c r="R5">
-        <v>32.5914784460354</v>
+        <v>32.2992252226806</v>
       </c>
       <c r="S5">
-        <v>33.7903443138264</v>
+        <v>30.8346113660416</v>
       </c>
       <c r="T5">
-        <v>82.3210368498612</v>
+        <v>81.9768821478371</v>
       </c>
       <c r="U5">
-        <v>3.81144624911056</v>
+        <v>3.17759358972222</v>
       </c>
       <c r="V5">
-        <v>7.57273914684919</v>
+        <v>9.25016903961268</v>
       </c>
       <c r="W5">
-        <v>2.70026624737487</v>
+        <v>3.47923476930583</v>
       </c>
       <c r="X5">
-        <v>4.91595493809455</v>
+        <v>3.34190152189813</v>
       </c>
       <c r="Y5">
-        <v>8.60836501272789</v>
+        <v>8.79643039198368</v>
       </c>
       <c r="Z5">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA5">
         <v>38400</v>
       </c>
       <c r="AB5">
-        <v>304.5744782524</v>
+        <v>298.736110537288</v>
       </c>
       <c r="AC5">
-        <v>553.314722222222</v>
+        <v>527.342638888889</v>
       </c>
       <c r="AD5">
-        <v>20329.9780217476</v>
+        <v>20357.0841672405</v>
       </c>
       <c r="AE5">
-        <v>18070.0219782524</v>
+        <v>18042.9158327595</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0.00159642401021711</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -951,61 +951,61 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0.00775088387272233</v>
+        <v>0.0067990209409845</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.283338663255516</v>
+        <v>0.278416347381865</v>
       </c>
       <c r="P6">
-        <v>30.5436544902969</v>
+        <v>32.6264185247354</v>
       </c>
       <c r="Q6">
-        <v>69.406320975634</v>
+        <v>69.5646243247223</v>
       </c>
       <c r="R6">
-        <v>32.0155027826491</v>
+        <v>31.6679917674393</v>
       </c>
       <c r="S6">
-        <v>33.4055026791674</v>
+        <v>30.2792756865068</v>
       </c>
       <c r="T6">
-        <v>81.0453271929147</v>
+        <v>80.5455115666195</v>
       </c>
       <c r="U6">
-        <v>3.79891569060393</v>
+        <v>3.09129012886463</v>
       </c>
       <c r="V6">
-        <v>7.52126535186663</v>
+        <v>9.07331281530734</v>
       </c>
       <c r="W6">
-        <v>2.66916975377326</v>
+        <v>3.43168568904769</v>
       </c>
       <c r="X6">
-        <v>4.87065306061356</v>
+        <v>3.25957677391981</v>
       </c>
       <c r="Y6">
-        <v>8.52598382872064</v>
+        <v>8.66223381950367</v>
       </c>
       <c r="Z6">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA6">
         <v>48000</v>
       </c>
       <c r="AB6">
-        <v>301.955810006408</v>
+        <v>295.356514468967</v>
       </c>
       <c r="AC6">
-        <v>8.53541666666667</v>
+        <v>2.60375</v>
       </c>
       <c r="AD6">
-        <v>20877.3759955491</v>
+        <v>20885.2026521977</v>
       </c>
       <c r="AE6">
-        <v>27122.6240044509</v>
+        <v>27114.7973478023</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.000319284802043423</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1046,61 +1046,61 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0.00027196083763938</v>
+        <v>0.00013598041881969</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0.0542957521558608</v>
+        <v>0.055874840357599</v>
       </c>
       <c r="P7">
-        <v>30.3091946913648</v>
+        <v>32.4246142298623</v>
       </c>
       <c r="Q7">
-        <v>68.8213141325306</v>
+        <v>69.0646560599087</v>
       </c>
       <c r="R7">
-        <v>31.8068886431536</v>
+        <v>31.3984739617419</v>
       </c>
       <c r="S7">
-        <v>33.0742065035481</v>
+        <v>29.8694418645876</v>
       </c>
       <c r="T7">
-        <v>80.4305303028662</v>
+        <v>79.9697483038763</v>
       </c>
       <c r="U7">
-        <v>3.7732313271428</v>
+        <v>3.0603735754767</v>
       </c>
       <c r="V7">
-        <v>7.46354392041806</v>
+        <v>8.95035178117271</v>
       </c>
       <c r="W7">
-        <v>2.63984312268841</v>
+        <v>3.40712230876119</v>
       </c>
       <c r="X7">
-        <v>4.85658045218995</v>
+        <v>3.24637844786093</v>
       </c>
       <c r="Y7">
-        <v>8.45914567635599</v>
+        <v>8.59499915469603</v>
       </c>
       <c r="Z7">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA7">
         <v>57600</v>
       </c>
       <c r="AB7">
-        <v>300.953425184167</v>
+        <v>294.226518834546</v>
       </c>
       <c r="AC7">
-        <v>4.14388888888889</v>
+        <v>2.60375</v>
       </c>
       <c r="AD7">
-        <v>20882.7699081492</v>
+        <v>20886.3326478321</v>
       </c>
       <c r="AE7">
-        <v>36717.2300918508</v>
+        <v>36713.6673521679</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.000543773790103317</v>
+        <v>0.000271886895051658</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1150,52 +1150,52 @@
         <v>0.00319284802043423</v>
       </c>
       <c r="P8">
-        <v>30.2701167364929</v>
+        <v>32.36706652199</v>
       </c>
       <c r="Q8">
-        <v>68.6661633916944</v>
+        <v>68.9532748682699</v>
       </c>
       <c r="R8">
-        <v>31.7474612221103</v>
+        <v>31.368157773898</v>
       </c>
       <c r="S8">
-        <v>32.9745154824147</v>
+        <v>29.783714812611</v>
       </c>
       <c r="T8">
-        <v>80.2628536639055</v>
+        <v>79.7346847524877</v>
       </c>
       <c r="U8">
-        <v>3.76125328987914</v>
+        <v>3.06009579769892</v>
       </c>
       <c r="V8">
-        <v>7.43430548906359</v>
+        <v>8.9424451681594</v>
       </c>
       <c r="W8">
-        <v>2.61743341013752</v>
+        <v>3.39880273118644</v>
       </c>
       <c r="X8">
-        <v>4.85230398923109</v>
+        <v>3.24637844786093</v>
       </c>
       <c r="Y8">
-        <v>8.36530925277783</v>
+        <v>8.53779072713542</v>
       </c>
       <c r="Z8">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA8">
         <v>67200</v>
       </c>
       <c r="AB8">
-        <v>300.670259905997</v>
+        <v>293.952537168908</v>
       </c>
       <c r="AC8">
-        <v>3.83319444444444</v>
+        <v>2.60375</v>
       </c>
       <c r="AD8">
-        <v>20883.3637678718</v>
+        <v>20886.6066294978</v>
       </c>
       <c r="AE8">
-        <v>46316.6362321282</v>
+        <v>46313.3933705022</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1215,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.000543773790103317</v>
+        <v>0.000271886895051658</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1245,52 +1245,52 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>30.2595582269145</v>
+        <v>32.360993478445</v>
       </c>
       <c r="Q9">
-        <v>68.6312551088603</v>
+        <v>68.9051064625343</v>
       </c>
       <c r="R9">
-        <v>31.7474612221103</v>
+        <v>31.3396421410115</v>
       </c>
       <c r="S9">
-        <v>32.9610971286904</v>
+        <v>29.7670336700955</v>
       </c>
       <c r="T9">
-        <v>80.2570505961771</v>
+        <v>79.705429937693</v>
       </c>
       <c r="U9">
-        <v>3.76125328987914</v>
+        <v>3.05105333030138</v>
       </c>
       <c r="V9">
-        <v>7.43430548906359</v>
+        <v>8.93282940238792</v>
       </c>
       <c r="W9">
-        <v>2.61743341013752</v>
+        <v>3.39880273118644</v>
       </c>
       <c r="X9">
-        <v>4.85230398923109</v>
+        <v>3.24637844786093</v>
       </c>
       <c r="Y9">
-        <v>8.36104307696242</v>
+        <v>8.53182369470614</v>
       </c>
       <c r="Z9">
-        <v>21187.8672222222</v>
+        <v>21183.1629166667</v>
       </c>
       <c r="AA9">
         <v>76800</v>
       </c>
       <c r="AB9">
-        <v>300.670259905997</v>
+        <v>293.824481613353</v>
       </c>
       <c r="AC9">
-        <v>3.83319444444444</v>
+        <v>2.60375</v>
       </c>
       <c r="AD9">
-        <v>20883.3637678718</v>
+        <v>20886.7346850533</v>
       </c>
       <c r="AE9">
-        <v>55916.6362321282</v>
+        <v>55913.2653149467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>